<commit_message>
basic functionality of journal entry completed
</commit_message>
<xml_diff>
--- a/data/testFile.xlsx
+++ b/data/testFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zenialau/Documents/GitHub/journal-entry-revamp/data/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>C</t>
   </si>
@@ -55,12 +55,31 @@
   </si>
   <si>
     <t>test 3 - debit and credit</t>
+  </si>
+  <si>
+    <t>Apr 1 - test 4</t>
+  </si>
+  <si>
+    <t>skdfjlj</t>
+  </si>
+  <si>
+    <t>test 5</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>test 6/7</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -426,40 +445,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D9514A-8EAF-9D4F-8653-791FEBA524DC}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>10.53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -469,15 +510,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784BFA4D-2623-1F45-B53E-5FC24EAEB496}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -487,24 +550,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202DD899-E015-3645-AC59-8A46B76EC854}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D1" t="n" s="0">
+        <v>37648.0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62012924-4E1B-2A4D-BD70-23A129538E39}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C1" t="n" s="0">
+        <v>37648.0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -519,17 +606,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="0">
         <v>10.53</v>
       </c>
     </row>

</xml_diff>